<commit_message>
probabilidade de ter 1 ou mais sintomas dado que o cara teve sintoma em qualquer intensidade
</commit_message>
<xml_diff>
--- a/conditional_prob_study1.xlsx
+++ b/conditional_prob_study1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e4b858b1fb629067/Documentos/sodium_bicarbonate_probabilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="8_{D8F7D2BA-572E-457D-A55B-2F3CD879DC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEA016A6-876F-4087-8F82-3401D0E05254}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{D8F7D2BA-572E-457D-A55B-2F3CD879DC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C18AE26A-EE8C-49FC-9AEF-CC465670D57E}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="-135" windowWidth="19470" windowHeight="14910" activeTab="1" xr2:uid="{2B0150EF-7BED-4B69-8ECF-8405627B5C69}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{2B0150EF-7BED-4B69-8ECF-8405627B5C69}"/>
   </bookViews>
   <sheets>
-    <sheet name="sintoma_severo" sheetId="1" r:id="rId1"/>
-    <sheet name="sintoma_mod" sheetId="2" r:id="rId2"/>
+    <sheet name="sintoma_any" sheetId="3" r:id="rId1"/>
+    <sheet name="sintoma_severo" sheetId="1" r:id="rId2"/>
+    <sheet name="sintoma_mod" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="46">
   <si>
     <t>Bryan</t>
   </si>
@@ -163,6 +164,18 @@
   </si>
   <si>
     <t>mais_2_sint_mod</t>
+  </si>
+  <si>
+    <t>soma_sintomas_any</t>
+  </si>
+  <si>
+    <t>teve_ao_menos_um_sint_any</t>
+  </si>
+  <si>
+    <t>mais_1_sint_any</t>
+  </si>
+  <si>
+    <t>mais_2_sint_any</t>
   </si>
 </sst>
 </file>
@@ -558,6 +571,4902 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5351F422-555A-430D-885E-35020A463B51}">
+  <dimension ref="A1:Z74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="23.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>SUM(C2:P2)</f>
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="str">
+        <f>IF(Q2&lt;&gt;0,"teve_sintoma_sev","não_teve_sintoma_sev")</f>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S2" s="1" t="str">
+        <f>IF(Q2&gt;1,"teve","não_teve")</f>
+        <v>teve</v>
+      </c>
+      <c r="T2" s="1" t="str">
+        <f>IF(Q2&gt;=3,"teve","não_teve")</f>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" ref="Q3:Q66" si="0">SUM(C3:P3)</f>
+        <v>1</v>
+      </c>
+      <c r="R3" s="1" t="str">
+        <f t="shared" ref="R3:R66" si="1">IF(Q3&lt;&gt;0,"teve_sintoma_sev","não_teve_sintoma_sev")</f>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S3" s="1" t="str">
+        <f t="shared" ref="S3:S66" si="2">IF(Q3&gt;1,"teve","não_teve")</f>
+        <v>não_teve</v>
+      </c>
+      <c r="T3" s="1" t="str">
+        <f t="shared" ref="T3:T66" si="3">IF(Q3&gt;=3,"teve","não_teve")</f>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T4" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T7" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T8" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T9" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T10" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="R13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T14" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="4"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="4"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="4"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="4"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="3">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="4"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="4"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="4"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="4"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0</v>
+      </c>
+      <c r="O24" s="3">
+        <v>0</v>
+      </c>
+      <c r="P24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="4"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3">
+        <v>0</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0</v>
+      </c>
+      <c r="P25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="4"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="4"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0</v>
+      </c>
+      <c r="P27" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="R27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="4"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="4"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="4"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
+        <v>1</v>
+      </c>
+      <c r="N30" s="3">
+        <v>0</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0</v>
+      </c>
+      <c r="P30" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="R30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30" s="5"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0</v>
+      </c>
+      <c r="N31" s="3">
+        <v>0</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0</v>
+      </c>
+      <c r="P31" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T31" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31" s="5"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <v>0</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0</v>
+      </c>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3">
+        <v>0</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T32" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32" s="5"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="3">
+        <v>0</v>
+      </c>
+      <c r="L33" s="3">
+        <v>0</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3">
+        <v>0</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0</v>
+      </c>
+      <c r="P33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T33" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+      <c r="Z33" s="5"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
+        <v>0</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0</v>
+      </c>
+      <c r="M34" s="3">
+        <v>1</v>
+      </c>
+      <c r="N34" s="3">
+        <v>0</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0</v>
+      </c>
+      <c r="P34" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T34" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34" s="5"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0</v>
+      </c>
+      <c r="L35" s="3">
+        <v>0</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+      <c r="N35" s="3">
+        <v>0</v>
+      </c>
+      <c r="O35" s="3">
+        <v>0</v>
+      </c>
+      <c r="P35" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="R35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T35" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35" s="5"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0</v>
+      </c>
+      <c r="L36" s="3">
+        <v>0</v>
+      </c>
+      <c r="M36" s="3">
+        <v>0</v>
+      </c>
+      <c r="N36" s="3">
+        <v>0</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0</v>
+      </c>
+      <c r="P36" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T36" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36" s="5"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>1</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0</v>
+      </c>
+      <c r="L37" s="3">
+        <v>0</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+      <c r="N37" s="3">
+        <v>0</v>
+      </c>
+      <c r="O37" s="3">
+        <v>0</v>
+      </c>
+      <c r="P37" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T37" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37" s="5"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3">
+        <v>0</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0</v>
+      </c>
+      <c r="N38" s="3">
+        <v>0</v>
+      </c>
+      <c r="O38" s="3">
+        <v>0</v>
+      </c>
+      <c r="P38" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S38" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T38" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+      <c r="Z38" s="5"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1</v>
+      </c>
+      <c r="J39" s="3">
+        <v>1</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0</v>
+      </c>
+      <c r="L39" s="3">
+        <v>0</v>
+      </c>
+      <c r="M39" s="3">
+        <v>0</v>
+      </c>
+      <c r="N39" s="3">
+        <v>0</v>
+      </c>
+      <c r="O39" s="3">
+        <v>0</v>
+      </c>
+      <c r="P39" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="R39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S39" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T39" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+      <c r="Z39" s="5"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0</v>
+      </c>
+      <c r="M40" s="3">
+        <v>0</v>
+      </c>
+      <c r="N40" s="3">
+        <v>0</v>
+      </c>
+      <c r="O40" s="3">
+        <v>0</v>
+      </c>
+      <c r="P40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S40" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T40" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40" s="5"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0</v>
+      </c>
+      <c r="L41" s="3">
+        <v>0</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+      <c r="N41" s="3">
+        <v>0</v>
+      </c>
+      <c r="O41" s="3">
+        <v>0</v>
+      </c>
+      <c r="P41" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S41" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T41" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+      <c r="Z41" s="5"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0</v>
+      </c>
+      <c r="J42" s="3">
+        <v>0</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" s="3">
+        <v>0</v>
+      </c>
+      <c r="M42" s="3">
+        <v>0</v>
+      </c>
+      <c r="N42" s="3">
+        <v>0</v>
+      </c>
+      <c r="O42" s="3">
+        <v>0</v>
+      </c>
+      <c r="P42" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S42" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T42" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+      <c r="Z42" s="5"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="L43" s="3">
+        <v>0</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+      <c r="N43" s="3">
+        <v>0</v>
+      </c>
+      <c r="O43" s="3">
+        <v>0</v>
+      </c>
+      <c r="P43" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R43" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S43" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T43" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+      <c r="U43"/>
+      <c r="V43"/>
+      <c r="W43"/>
+      <c r="X43"/>
+      <c r="Y43"/>
+      <c r="Z43" s="5"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3">
+        <v>1</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0</v>
+      </c>
+      <c r="N44" s="3">
+        <v>0</v>
+      </c>
+      <c r="O44" s="3">
+        <v>0</v>
+      </c>
+      <c r="P44" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R44" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S44" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T44" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0</v>
+      </c>
+      <c r="L45" s="3">
+        <v>0</v>
+      </c>
+      <c r="M45" s="3">
+        <v>0</v>
+      </c>
+      <c r="N45" s="3">
+        <v>0</v>
+      </c>
+      <c r="O45" s="3">
+        <v>0</v>
+      </c>
+      <c r="P45" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R45" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S45" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T45" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+      <c r="K46" s="3">
+        <v>0</v>
+      </c>
+      <c r="L46" s="3">
+        <v>0</v>
+      </c>
+      <c r="M46" s="3">
+        <v>0</v>
+      </c>
+      <c r="N46" s="3">
+        <v>0</v>
+      </c>
+      <c r="O46" s="3">
+        <v>0</v>
+      </c>
+      <c r="P46" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R46" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S46" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T46" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0</v>
+      </c>
+      <c r="L47" s="3">
+        <v>0</v>
+      </c>
+      <c r="M47" s="3">
+        <v>0</v>
+      </c>
+      <c r="N47" s="3">
+        <v>0</v>
+      </c>
+      <c r="O47" s="3">
+        <v>0</v>
+      </c>
+      <c r="P47" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R47" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S47" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T47" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>1</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0</v>
+      </c>
+      <c r="L48" s="3">
+        <v>0</v>
+      </c>
+      <c r="M48" s="3">
+        <v>0</v>
+      </c>
+      <c r="N48" s="3">
+        <v>0</v>
+      </c>
+      <c r="O48" s="3">
+        <v>0</v>
+      </c>
+      <c r="P48" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R48" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S48" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T48" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1</v>
+      </c>
+      <c r="J49" s="3">
+        <v>0</v>
+      </c>
+      <c r="K49" s="3">
+        <v>0</v>
+      </c>
+      <c r="L49" s="3">
+        <v>0</v>
+      </c>
+      <c r="M49" s="3">
+        <v>0</v>
+      </c>
+      <c r="N49" s="3">
+        <v>0</v>
+      </c>
+      <c r="O49" s="3">
+        <v>0</v>
+      </c>
+      <c r="P49" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R49" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S49" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T49" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3">
+        <v>0</v>
+      </c>
+      <c r="L50" s="3">
+        <v>0</v>
+      </c>
+      <c r="M50" s="3">
+        <v>0</v>
+      </c>
+      <c r="N50" s="3">
+        <v>0</v>
+      </c>
+      <c r="O50" s="3">
+        <v>0</v>
+      </c>
+      <c r="P50" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R50" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S50" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T50" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+      <c r="J51" s="3">
+        <v>0</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0</v>
+      </c>
+      <c r="L51" s="3">
+        <v>0</v>
+      </c>
+      <c r="M51" s="3">
+        <v>0</v>
+      </c>
+      <c r="N51" s="3">
+        <v>0</v>
+      </c>
+      <c r="O51" s="3">
+        <v>0</v>
+      </c>
+      <c r="P51" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R51" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S51" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T51" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3">
+        <v>0</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0</v>
+      </c>
+      <c r="L52" s="3">
+        <v>0</v>
+      </c>
+      <c r="M52" s="3">
+        <v>0</v>
+      </c>
+      <c r="N52" s="3">
+        <v>0</v>
+      </c>
+      <c r="O52" s="3">
+        <v>0</v>
+      </c>
+      <c r="P52" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R52" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S52" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T52" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3">
+        <v>1</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <v>0</v>
+      </c>
+      <c r="J53" s="3">
+        <v>0</v>
+      </c>
+      <c r="K53" s="3">
+        <v>0</v>
+      </c>
+      <c r="L53" s="3">
+        <v>0</v>
+      </c>
+      <c r="M53" s="3">
+        <v>0</v>
+      </c>
+      <c r="N53" s="3">
+        <v>0</v>
+      </c>
+      <c r="O53" s="3">
+        <v>0</v>
+      </c>
+      <c r="P53" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R53" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S53" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T53" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>1</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3">
+        <v>1</v>
+      </c>
+      <c r="J54" s="3">
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0</v>
+      </c>
+      <c r="L54" s="3">
+        <v>0</v>
+      </c>
+      <c r="M54" s="3">
+        <v>0</v>
+      </c>
+      <c r="N54" s="3">
+        <v>0</v>
+      </c>
+      <c r="O54" s="3">
+        <v>0</v>
+      </c>
+      <c r="P54" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="R54" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S54" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T54" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3">
+        <v>1</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>1</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <v>1</v>
+      </c>
+      <c r="L55" s="3">
+        <v>0</v>
+      </c>
+      <c r="M55" s="3">
+        <v>0</v>
+      </c>
+      <c r="N55" s="3">
+        <v>0</v>
+      </c>
+      <c r="O55" s="3">
+        <v>0</v>
+      </c>
+      <c r="P55" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="R55" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S55" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T55" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0</v>
+      </c>
+      <c r="L56" s="3">
+        <v>0</v>
+      </c>
+      <c r="M56" s="3">
+        <v>0</v>
+      </c>
+      <c r="N56" s="3">
+        <v>0</v>
+      </c>
+      <c r="O56" s="3">
+        <v>0</v>
+      </c>
+      <c r="P56" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R56" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S56" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T56" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="3">
+        <v>1</v>
+      </c>
+      <c r="D57" s="3">
+        <v>1</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3">
+        <v>1</v>
+      </c>
+      <c r="H57" s="3">
+        <v>1</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0</v>
+      </c>
+      <c r="J57" s="3">
+        <v>0</v>
+      </c>
+      <c r="K57" s="3">
+        <v>1</v>
+      </c>
+      <c r="L57" s="3">
+        <v>1</v>
+      </c>
+      <c r="M57" s="3">
+        <v>0</v>
+      </c>
+      <c r="N57" s="3">
+        <v>1</v>
+      </c>
+      <c r="O57" s="3">
+        <v>0</v>
+      </c>
+      <c r="P57" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="R57" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S57" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T57" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3">
+        <v>1</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3">
+        <v>1</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3">
+        <v>1</v>
+      </c>
+      <c r="J58" s="3">
+        <v>0</v>
+      </c>
+      <c r="K58" s="3">
+        <v>0</v>
+      </c>
+      <c r="L58" s="3">
+        <v>0</v>
+      </c>
+      <c r="M58" s="3">
+        <v>0</v>
+      </c>
+      <c r="N58" s="3">
+        <v>0</v>
+      </c>
+      <c r="O58" s="3">
+        <v>0</v>
+      </c>
+      <c r="P58" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="R58" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S58" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>teve</v>
+      </c>
+      <c r="T58" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>teve</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="3">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
+      <c r="J59" s="3">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3">
+        <v>0</v>
+      </c>
+      <c r="L59" s="3">
+        <v>0</v>
+      </c>
+      <c r="M59" s="3">
+        <v>0</v>
+      </c>
+      <c r="N59" s="3">
+        <v>0</v>
+      </c>
+      <c r="O59" s="3">
+        <v>0</v>
+      </c>
+      <c r="P59" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R59" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S59" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T59" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="3">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0</v>
+      </c>
+      <c r="E60" s="3">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <v>0</v>
+      </c>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
+      <c r="I60" s="3">
+        <v>1</v>
+      </c>
+      <c r="J60" s="3">
+        <v>0</v>
+      </c>
+      <c r="K60" s="3">
+        <v>0</v>
+      </c>
+      <c r="L60" s="3">
+        <v>0</v>
+      </c>
+      <c r="M60" s="3">
+        <v>0</v>
+      </c>
+      <c r="N60" s="3">
+        <v>0</v>
+      </c>
+      <c r="O60" s="3">
+        <v>0</v>
+      </c>
+      <c r="P60" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R60" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S60" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T60" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="3">
+        <v>0</v>
+      </c>
+      <c r="D61" s="3">
+        <v>0</v>
+      </c>
+      <c r="E61" s="3">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3">
+        <v>0</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0</v>
+      </c>
+      <c r="J61" s="3">
+        <v>0</v>
+      </c>
+      <c r="K61" s="3">
+        <v>0</v>
+      </c>
+      <c r="L61" s="3">
+        <v>0</v>
+      </c>
+      <c r="M61" s="3">
+        <v>0</v>
+      </c>
+      <c r="N61" s="3">
+        <v>0</v>
+      </c>
+      <c r="O61" s="3">
+        <v>0</v>
+      </c>
+      <c r="P61" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R61" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S61" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T61" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>0</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0</v>
+      </c>
+      <c r="J62" s="3">
+        <v>0</v>
+      </c>
+      <c r="K62" s="3">
+        <v>0</v>
+      </c>
+      <c r="L62" s="3">
+        <v>0</v>
+      </c>
+      <c r="M62" s="3">
+        <v>0</v>
+      </c>
+      <c r="N62" s="3">
+        <v>0</v>
+      </c>
+      <c r="O62" s="3">
+        <v>0</v>
+      </c>
+      <c r="P62" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R62" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S62" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T62" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0</v>
+      </c>
+      <c r="E63" s="3">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3">
+        <v>0</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="I63" s="3">
+        <v>0</v>
+      </c>
+      <c r="J63" s="3">
+        <v>0</v>
+      </c>
+      <c r="K63" s="3">
+        <v>0</v>
+      </c>
+      <c r="L63" s="3">
+        <v>0</v>
+      </c>
+      <c r="M63" s="3">
+        <v>0</v>
+      </c>
+      <c r="N63" s="3">
+        <v>0</v>
+      </c>
+      <c r="O63" s="3">
+        <v>0</v>
+      </c>
+      <c r="P63" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R63" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S63" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T63" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="3">
+        <v>0</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="3">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3">
+        <v>0</v>
+      </c>
+      <c r="G64" s="3">
+        <v>0</v>
+      </c>
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3">
+        <v>1</v>
+      </c>
+      <c r="J64" s="3">
+        <v>0</v>
+      </c>
+      <c r="K64" s="3">
+        <v>0</v>
+      </c>
+      <c r="L64" s="3">
+        <v>0</v>
+      </c>
+      <c r="M64" s="3">
+        <v>0</v>
+      </c>
+      <c r="N64" s="3">
+        <v>0</v>
+      </c>
+      <c r="O64" s="3">
+        <v>0</v>
+      </c>
+      <c r="P64" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R64" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S64" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T64" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0</v>
+      </c>
+      <c r="E65" s="3">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3">
+        <v>0</v>
+      </c>
+      <c r="J65" s="3">
+        <v>0</v>
+      </c>
+      <c r="K65" s="3">
+        <v>0</v>
+      </c>
+      <c r="L65" s="3">
+        <v>0</v>
+      </c>
+      <c r="M65" s="3">
+        <v>0</v>
+      </c>
+      <c r="N65" s="3">
+        <v>0</v>
+      </c>
+      <c r="O65" s="3">
+        <v>0</v>
+      </c>
+      <c r="P65" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R65" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S65" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T65" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" s="3">
+        <v>0</v>
+      </c>
+      <c r="D66" s="3">
+        <v>0</v>
+      </c>
+      <c r="E66" s="3">
+        <v>0</v>
+      </c>
+      <c r="F66" s="3">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3">
+        <v>0</v>
+      </c>
+      <c r="I66" s="3">
+        <v>0</v>
+      </c>
+      <c r="J66" s="3">
+        <v>0</v>
+      </c>
+      <c r="K66" s="3">
+        <v>0</v>
+      </c>
+      <c r="L66" s="3">
+        <v>0</v>
+      </c>
+      <c r="M66" s="3">
+        <v>0</v>
+      </c>
+      <c r="N66" s="3">
+        <v>0</v>
+      </c>
+      <c r="O66" s="3">
+        <v>0</v>
+      </c>
+      <c r="P66" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R66" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S66" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T66" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C67" s="3">
+        <v>0</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3">
+        <v>0</v>
+      </c>
+      <c r="F67" s="3">
+        <v>0</v>
+      </c>
+      <c r="G67" s="3">
+        <v>0</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>0</v>
+      </c>
+      <c r="J67" s="3">
+        <v>0</v>
+      </c>
+      <c r="K67" s="3">
+        <v>0</v>
+      </c>
+      <c r="L67" s="3">
+        <v>0</v>
+      </c>
+      <c r="M67" s="3">
+        <v>0</v>
+      </c>
+      <c r="N67" s="3">
+        <v>0</v>
+      </c>
+      <c r="O67" s="3">
+        <v>0</v>
+      </c>
+      <c r="P67" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="1">
+        <f t="shared" ref="Q67:Q71" si="4">SUM(C67:P67)</f>
+        <v>0</v>
+      </c>
+      <c r="R67" s="1" t="str">
+        <f t="shared" ref="R67:R71" si="5">IF(Q67&lt;&gt;0,"teve_sintoma_sev","não_teve_sintoma_sev")</f>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S67" s="1" t="str">
+        <f t="shared" ref="S67:S71" si="6">IF(Q67&gt;1,"teve","não_teve")</f>
+        <v>não_teve</v>
+      </c>
+      <c r="T67" s="1" t="str">
+        <f t="shared" ref="T67:T71" si="7">IF(Q67&gt;=3,"teve","não_teve")</f>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="3">
+        <v>0</v>
+      </c>
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
+      <c r="E68" s="3">
+        <v>0</v>
+      </c>
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
+      <c r="G68" s="3">
+        <v>1</v>
+      </c>
+      <c r="H68" s="3">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3">
+        <v>1</v>
+      </c>
+      <c r="J68" s="3">
+        <v>0</v>
+      </c>
+      <c r="K68" s="3">
+        <v>0</v>
+      </c>
+      <c r="L68" s="3">
+        <v>0</v>
+      </c>
+      <c r="M68" s="3">
+        <v>0</v>
+      </c>
+      <c r="N68" s="3">
+        <v>0</v>
+      </c>
+      <c r="O68" s="3">
+        <v>0</v>
+      </c>
+      <c r="P68" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="1">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="R68" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S68" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>teve</v>
+      </c>
+      <c r="T68" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" s="3">
+        <v>0</v>
+      </c>
+      <c r="D69" s="3">
+        <v>0</v>
+      </c>
+      <c r="E69" s="3">
+        <v>0</v>
+      </c>
+      <c r="F69" s="3">
+        <v>0</v>
+      </c>
+      <c r="G69" s="3">
+        <v>0</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
+      <c r="I69" s="3">
+        <v>0</v>
+      </c>
+      <c r="J69" s="3">
+        <v>0</v>
+      </c>
+      <c r="K69" s="3">
+        <v>1</v>
+      </c>
+      <c r="L69" s="3">
+        <v>0</v>
+      </c>
+      <c r="M69" s="3">
+        <v>0</v>
+      </c>
+      <c r="N69" s="3">
+        <v>0</v>
+      </c>
+      <c r="O69" s="3">
+        <v>0</v>
+      </c>
+      <c r="P69" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="R69" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>teve_sintoma_sev</v>
+      </c>
+      <c r="S69" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T69" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="3">
+        <v>0</v>
+      </c>
+      <c r="D70" s="3">
+        <v>0</v>
+      </c>
+      <c r="E70" s="3">
+        <v>0</v>
+      </c>
+      <c r="F70" s="3">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3">
+        <v>0</v>
+      </c>
+      <c r="H70" s="3">
+        <v>0</v>
+      </c>
+      <c r="I70" s="3">
+        <v>0</v>
+      </c>
+      <c r="J70" s="3">
+        <v>0</v>
+      </c>
+      <c r="K70" s="3">
+        <v>0</v>
+      </c>
+      <c r="L70" s="3">
+        <v>0</v>
+      </c>
+      <c r="M70" s="3">
+        <v>0</v>
+      </c>
+      <c r="N70" s="3">
+        <v>0</v>
+      </c>
+      <c r="O70" s="3">
+        <v>0</v>
+      </c>
+      <c r="P70" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R70" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S70" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T70" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="3">
+        <v>0</v>
+      </c>
+      <c r="D71" s="3">
+        <v>0</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3">
+        <v>0</v>
+      </c>
+      <c r="G71" s="3">
+        <v>0</v>
+      </c>
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
+      <c r="I71" s="3">
+        <v>0</v>
+      </c>
+      <c r="J71" s="3">
+        <v>0</v>
+      </c>
+      <c r="K71" s="3">
+        <v>0</v>
+      </c>
+      <c r="L71" s="3">
+        <v>0</v>
+      </c>
+      <c r="M71" s="3">
+        <v>0</v>
+      </c>
+      <c r="N71" s="3">
+        <v>0</v>
+      </c>
+      <c r="O71" s="3">
+        <v>0</v>
+      </c>
+      <c r="P71" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R71" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>não_teve_sintoma_sev</v>
+      </c>
+      <c r="S71" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>não_teve</v>
+      </c>
+      <c r="T71" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>não_teve</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N72"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R73" s="6"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R74" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9572D4E4-F17F-47B0-8DB0-491D5EA53248}">
   <dimension ref="A1:Z74"/>
   <sheetViews>
@@ -5451,11 +10360,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AD602E-5543-49F4-AD06-4A2A40345688}">
   <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tabela com dados de qualquer sintoma
</commit_message>
<xml_diff>
--- a/conditional_prob_study1.xlsx
+++ b/conditional_prob_study1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e4b858b1fb629067/Documentos/sodium_bicarbonate_probabilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{D8F7D2BA-572E-457D-A55B-2F3CD879DC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C18AE26A-EE8C-49FC-9AEF-CC465670D57E}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{D8F7D2BA-572E-457D-A55B-2F3CD879DC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2086D061-AD24-4FB4-B025-159CCCE04237}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{2B0150EF-7BED-4B69-8ECF-8405627B5C69}"/>
   </bookViews>
@@ -575,7 +575,7 @@
   <dimension ref="A1:Z74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>